<commit_message>
Kleine Korrekturen + Deckblatt
Fehlerbetrachtung fehlt
</commit_message>
<xml_diff>
--- a/V1.2/data/Messwerte V1.2.xlsx
+++ b/V1.2/data/Messwerte V1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Studium\Analytik_Protokolle\V1.2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0830B1DD-64F0-4C89-9FA9-8A71D946DCBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF893247-73B9-4E58-B9B0-A3135271ABDE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -270,7 +270,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -279,7 +278,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3704,8 +3703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF216252-ABA1-A14F-BC57-E20FE8A85DB6}">
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,19 +3756,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>0</v>
       </c>
       <c r="B3">
         <v>545</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>0</v>
       </c>
       <c r="D3">
         <v>545</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <f t="shared" ref="E3:E43" si="0">C3</f>
         <v>0</v>
       </c>
@@ -3803,21 +3802,21 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <f t="shared" ref="A4:A43" si="1">A3+0.5</f>
         <v>0.5</v>
       </c>
       <c r="B4">
         <v>543</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <f t="shared" ref="C4:C43" si="2">C3+0.5</f>
         <v>0.5</v>
       </c>
       <c r="D4">
         <v>544</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -3847,21 +3846,21 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B5">
         <v>540</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="D5">
         <v>541</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3891,21 +3890,21 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
       <c r="B6">
         <v>537</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
       <c r="D6">
         <v>538</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
@@ -3914,21 +3913,21 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="B7">
         <v>534</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="D7">
         <v>535</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3958,21 +3957,21 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
       <c r="B8">
         <v>532</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
       <c r="D8">
         <v>533</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -4002,21 +4001,21 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="B9">
         <v>529</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="D9">
         <v>530</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -4046,21 +4045,21 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
       <c r="B10">
         <v>526</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="D10">
         <v>527</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
@@ -4073,21 +4072,21 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="8">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B11">
         <v>524</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="D11">
         <v>525</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -4108,21 +4107,21 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
       <c r="B12">
         <v>521</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
       <c r="D12">
         <v>522</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
@@ -4133,7 +4132,7 @@
         <f>AVERAGE(O7:O9)</f>
         <v>25.243105708016284</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <f>_xlfn.STDEV.S(O7:O9)</f>
         <v>5.3351161595554003E-2</v>
       </c>
@@ -4141,27 +4140,27 @@
         <f>COUNT(O7:O9)</f>
         <v>3</v>
       </c>
-      <c r="M12" s="8">
+      <c r="M12" s="4">
         <f>K12*2.92/SQRT(3)</f>
         <v>8.9942737925615204E-2</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B13">
         <v>518</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="D13">
         <v>520</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -4170,21 +4169,21 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
       <c r="B14">
         <v>516</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="8">
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
       <c r="D14">
         <v>517</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
@@ -4195,27 +4194,27 @@
         <f>409-544</f>
         <v>-135</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M14" s="7">
         <f>(J12-250)/K12*SQRT(L12)</f>
         <v>-7296.7550962853729</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B15">
         <v>514</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="D15">
         <v>515</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -4228,21 +4227,21 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
       <c r="B16">
         <v>511</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="8">
         <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
       <c r="D16">
         <v>513</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
@@ -4255,21 +4254,21 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B17" s="1">
         <v>510</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="D17" s="1">
         <v>511</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -4278,21 +4277,21 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
       <c r="B18">
         <v>512</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="8">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
       <c r="D18">
         <v>514</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -4308,21 +4307,21 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B19">
         <v>518</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="D19">
         <v>520</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -4338,21 +4337,21 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
       <c r="B20">
         <v>526</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
       <c r="D20">
         <v>528</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
@@ -4368,21 +4367,21 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B21">
         <v>533</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="D21">
         <v>535</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -4398,21 +4397,21 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
       <c r="B22">
         <v>540</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="8">
         <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
       <c r="D22">
         <v>543</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="8">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
@@ -4428,21 +4427,21 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B23">
         <v>548</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="D23">
         <v>551</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -4458,21 +4457,21 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9">
+      <c r="A24" s="8">
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
       <c r="B24">
         <v>555</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <f t="shared" si="2"/>
         <v>10.5</v>
       </c>
       <c r="D24">
         <v>558</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
@@ -4481,21 +4480,21 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="9">
+      <c r="A25" s="8">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B25">
         <v>563</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="8">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="D25">
         <v>565</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
@@ -4504,21 +4503,21 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9">
+      <c r="A26" s="8">
         <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
       <c r="B26">
         <v>570</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <f t="shared" si="2"/>
         <v>11.5</v>
       </c>
       <c r="D26">
         <v>573</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <f t="shared" si="0"/>
         <v>11.5</v>
       </c>
@@ -4527,21 +4526,21 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="9">
+      <c r="A27" s="8">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B27">
         <v>577</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="D27">
         <v>580</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -4550,21 +4549,21 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="9">
+      <c r="A28" s="8">
         <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
       <c r="B28">
         <v>585</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
       <c r="D28">
         <v>587</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
@@ -4573,21 +4572,21 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="9">
+      <c r="A29" s="8">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B29">
         <v>592</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="D29">
         <v>595</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -4596,21 +4595,21 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
+      <c r="A30" s="8">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
       <c r="B30">
         <v>599</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <f t="shared" si="2"/>
         <v>13.5</v>
       </c>
       <c r="D30">
         <v>602</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <f t="shared" si="0"/>
         <v>13.5</v>
       </c>
@@ -4619,21 +4618,21 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
+      <c r="A31" s="8">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B31">
         <v>606</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="D31">
         <v>609</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="8">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -4642,21 +4641,21 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
+      <c r="A32" s="8">
         <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
       <c r="B32">
         <v>613</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <f t="shared" si="2"/>
         <v>14.5</v>
       </c>
       <c r="D32">
         <v>616</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
@@ -4665,21 +4664,21 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="9">
+      <c r="A33" s="8">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B33">
         <v>620</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="D33">
         <v>623</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -4688,21 +4687,21 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9">
+      <c r="A34" s="8">
         <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
       <c r="B34">
         <v>626</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <f t="shared" si="2"/>
         <v>15.5</v>
       </c>
       <c r="D34">
         <v>630</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="8">
         <f t="shared" si="0"/>
         <v>15.5</v>
       </c>
@@ -4711,21 +4710,21 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="9">
+      <c r="A35" s="8">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B35">
         <v>633</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="D35">
         <v>636</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -4734,21 +4733,21 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9">
+      <c r="A36" s="8">
         <f t="shared" si="1"/>
         <v>16.5</v>
       </c>
       <c r="B36">
         <v>640</v>
       </c>
-      <c r="C36" s="9">
+      <c r="C36" s="8">
         <f t="shared" si="2"/>
         <v>16.5</v>
       </c>
       <c r="D36">
         <v>643</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="8">
         <f t="shared" si="0"/>
         <v>16.5</v>
       </c>
@@ -4757,21 +4756,21 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="9">
+      <c r="A37" s="8">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B37">
         <v>647</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="D37">
         <v>650</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="8">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -4780,21 +4779,21 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9">
+      <c r="A38" s="8">
         <f t="shared" si="1"/>
         <v>17.5</v>
       </c>
       <c r="B38">
         <v>653</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="D38">
         <v>657</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="8">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
@@ -4803,21 +4802,21 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9">
+      <c r="A39" s="8">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B39">
         <v>660</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="D39">
         <v>663</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="8">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -4826,21 +4825,21 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="9">
+      <c r="A40" s="8">
         <f t="shared" si="1"/>
         <v>18.5</v>
       </c>
       <c r="B40">
         <v>666</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <f t="shared" si="2"/>
         <v>18.5</v>
       </c>
       <c r="D40">
         <v>670</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="8">
         <f t="shared" si="0"/>
         <v>18.5</v>
       </c>
@@ -4849,21 +4848,21 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="9">
+      <c r="A41" s="8">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B41">
         <v>673</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="8">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="D41">
         <v>676</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="8">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -4872,21 +4871,21 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="9">
+      <c r="A42" s="8">
         <f t="shared" si="1"/>
         <v>19.5</v>
       </c>
       <c r="B42">
         <v>679</v>
       </c>
-      <c r="C42" s="9">
+      <c r="C42" s="8">
         <f t="shared" si="2"/>
         <v>19.5</v>
       </c>
       <c r="D42">
         <v>683</v>
       </c>
-      <c r="E42" s="9">
+      <c r="E42" s="8">
         <f t="shared" si="0"/>
         <v>19.5</v>
       </c>
@@ -4895,21 +4894,21 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9">
+      <c r="A43" s="8">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B43">
         <v>685</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C43" s="8">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="D43">
         <v>689</v>
       </c>
-      <c r="E43" s="9">
+      <c r="E43" s="8">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -4928,7 +4927,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4978,7 +4977,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>0</v>
       </c>
       <c r="B3">
@@ -4987,7 +4986,7 @@
       <c r="C3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>0</v>
       </c>
       <c r="E3">
@@ -4996,7 +4995,7 @@
       <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <f t="shared" ref="G3:G23" si="0">D3</f>
         <v>0</v>
       </c>
@@ -5022,7 +5021,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <f t="shared" ref="A4:A23" si="1">A3+0.5</f>
         <v>0.5</v>
       </c>
@@ -5033,7 +5032,7 @@
         <f>B4-B3</f>
         <v>8</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <f t="shared" ref="D4:D23" si="2">D3+0.5</f>
         <v>0.5</v>
       </c>
@@ -5044,7 +5043,7 @@
         <f>E4-E3</f>
         <v>3</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
@@ -5071,7 +5070,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="8">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -5082,7 +5081,7 @@
         <f t="shared" ref="C5:C23" si="3">B5-B4</f>
         <v>5</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -5093,7 +5092,7 @@
         <f t="shared" ref="F5:F23" si="4">E5-E4</f>
         <v>5</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -5113,7 +5112,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="8">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
@@ -5124,7 +5123,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
@@ -5135,7 +5134,7 @@
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
@@ -5155,7 +5154,7 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="8">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -5166,7 +5165,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -5177,7 +5176,7 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -5204,7 +5203,7 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="A8" s="8">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
@@ -5215,7 +5214,7 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
@@ -5226,7 +5225,7 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
@@ -5253,7 +5252,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -5264,7 +5263,7 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
@@ -5275,7 +5274,7 @@
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -5299,7 +5298,7 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
@@ -5310,7 +5309,7 @@
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
@@ -5321,7 +5320,7 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
@@ -5342,7 +5341,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="10">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
@@ -5353,7 +5352,7 @@
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="10">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
@@ -5364,7 +5363,7 @@
         <f t="shared" si="4"/>
         <v>51</v>
       </c>
-      <c r="G11" s="11">
+      <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -5391,7 +5390,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="A12" s="8">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
@@ -5402,7 +5401,7 @@
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <f t="shared" si="2"/>
         <v>4.5</v>
       </c>
@@ -5413,7 +5412,7 @@
         <f t="shared" si="4"/>
         <v>21</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
@@ -5440,7 +5439,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -5451,7 +5450,7 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
@@ -5462,7 +5461,7 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
@@ -5482,7 +5481,7 @@
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
@@ -5493,7 +5492,7 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
@@ -5504,7 +5503,7 @@
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="8">
         <f t="shared" si="0"/>
         <v>5.5</v>
       </c>
@@ -5517,7 +5516,7 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
+      <c r="A15" s="8">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -5528,7 +5527,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
@@ -5539,7 +5538,7 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -5559,7 +5558,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="A16" s="8">
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
@@ -5570,7 +5569,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="8">
         <f t="shared" si="2"/>
         <v>6.5</v>
       </c>
@@ -5581,7 +5580,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="8">
         <f t="shared" si="0"/>
         <v>6.5</v>
       </c>
@@ -5601,7 +5600,7 @@
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="11">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
@@ -5612,7 +5611,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -5623,7 +5622,7 @@
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
@@ -5643,7 +5642,7 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="9">
+      <c r="A18" s="8">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
@@ -5654,7 +5653,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="8">
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
@@ -5665,7 +5664,7 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="8">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -5678,7 +5677,7 @@
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="9">
+      <c r="A19" s="8">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -5689,7 +5688,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -5700,7 +5699,7 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
@@ -5714,10 +5713,10 @@
       <c r="M19" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="N19" s="13" t="s">
+      <c r="N19" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="O19" s="13"/>
+      <c r="O19" s="12"/>
       <c r="P19" s="6" t="s">
         <v>22</v>
       </c>
@@ -5729,7 +5728,7 @@
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="A20" s="8">
         <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
@@ -5740,7 +5739,7 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
@@ -5751,7 +5750,7 @@
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
@@ -5766,26 +5765,26 @@
         <f>AVERAGE(N15:N17)</f>
         <v>25.9256639594246</v>
       </c>
-      <c r="N20" s="14">
+      <c r="N20" s="13">
         <f>_xlfn.STDEV.S(N15:N17)</f>
         <v>6.3670836642459094E-2</v>
       </c>
-      <c r="O20" s="14"/>
+      <c r="O20" s="13"/>
       <c r="P20">
         <f>COUNT(N15:N17)</f>
         <v>3</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="4">
         <f>2.92/SQRT(3)*N20</f>
         <v>0.10734029405115314</v>
       </c>
-      <c r="R20" s="8">
+      <c r="R20" s="7">
         <f>(M20-250)/N20*SQRT(P20)</f>
         <v>-6095.5400487972765</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="A21" s="8">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -5796,7 +5795,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
@@ -5807,7 +5806,7 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -5820,7 +5819,7 @@
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="9">
+      <c r="A22" s="8">
         <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
@@ -5831,7 +5830,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <f t="shared" si="2"/>
         <v>9.5</v>
       </c>
@@ -5842,7 +5841,7 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="8">
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
@@ -5855,7 +5854,7 @@
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="9">
+      <c r="A23" s="8">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -5866,7 +5865,7 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="8">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -5877,7 +5876,7 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="8">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>

</xml_diff>